<commit_message>
Formats ano had 2017
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RAPSS ANO 17.xlsx
+++ b/formats/excel/Formats RAPSS ANO 17.xlsx
@@ -642,19 +642,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,24 +672,26 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -716,7 +711,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -737,10 +740,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -760,55 +772,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -824,6 +789,28 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -856,7 +843,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,175 +1023,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1091,6 +1078,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1125,6 +1127,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1150,36 +1167,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1193,145 +1180,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1345,45 +1332,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1702,9 +1689,9 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -2750,7 +2737,9 @@
       <c r="E52" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="10">
@@ -2768,7 +2757,9 @@
       <c r="E53" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F53" s="2"/>
+      <c r="F53" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="10">
@@ -2786,7 +2777,9 @@
       <c r="E54" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="10">
@@ -2804,7 +2797,9 @@
       <c r="E55" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F55" s="2"/>
+      <c r="F55" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="10">
@@ -2822,7 +2817,9 @@
       <c r="E56" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F56" s="2"/>
+      <c r="F56" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="10">
@@ -2840,7 +2837,9 @@
       <c r="E57" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="10">
@@ -2858,7 +2857,9 @@
       <c r="E58" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="F58" s="2"/>
+      <c r="F58" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="10">
@@ -2876,7 +2877,9 @@
       <c r="E59" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="F59" s="2"/>
+      <c r="F59" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="10">
@@ -2894,7 +2897,9 @@
       <c r="E60" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="F60" s="2"/>
+      <c r="F60" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="10">
@@ -2912,7 +2917,9 @@
       <c r="E61" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="F61" s="2"/>
+      <c r="F61" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="12">

</xml_diff>

<commit_message>
formats had ano %>% ok
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RAPSS ANO 17.xlsx
+++ b/formats/excel/Formats RAPSS ANO 17.xlsx
@@ -642,9 +642,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -695,48 +695,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -748,17 +711,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -788,16 +756,41 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -810,7 +803,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -849,13 +849,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,73 +891,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -951,13 +921,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -969,25 +981,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -999,31 +1023,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1097,15 +1097,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -1141,6 +1132,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1158,10 +1160,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1180,139 +1180,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1691,7 +1691,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F104" sqref="F104"/>
+      <selection pane="bottomLeft" activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -3692,7 +3692,7 @@
         <v>417</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="E100" s="16" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
Ajout des med et um ssr
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RAPSS ANO 17.xlsx
+++ b/formats/excel/Formats RAPSS ANO 17.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208">
   <si>
     <t>longueur</t>
   </si>
@@ -623,6 +623,9 @@
   </si>
   <si>
     <t>Date de sortie</t>
+  </si>
+  <si>
+    <t>Filler4</t>
   </si>
   <si>
     <t>EMPNUM</t>
@@ -642,10 +645,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -680,16 +683,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -704,15 +722,23 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,7 +752,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -741,15 +790,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -763,16 +804,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -781,36 +814,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -849,13 +852,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,37 +918,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,7 +936,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,25 +972,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -963,25 +996,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -993,37 +1026,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1097,22 +1100,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1134,11 +1122,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1158,10 +1144,27 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1180,142 +1183,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -1691,7 +1694,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D101" sqref="D101"/>
+      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -3692,7 +3695,7 @@
         <v>417</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="E100" s="16" t="s">
         <v>83</v>
@@ -3712,10 +3715,10 @@
         <v>449</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E101" s="16" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F101" t="s">
         <v>8</v>
@@ -3732,10 +3735,10 @@
         <v>793</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E102" s="16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F102" t="s">
         <v>8</v>

</xml_diff>